<commit_message>
Callers-to-Coders upd - 6.25.20
Callers-to-Coders upd - 6.25.20
</commit_message>
<xml_diff>
--- a/Examples/Data Dictionary - Covid-19.xlsx
+++ b/Examples/Data Dictionary - Covid-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JTB Ventures LLC\Documents\GitHub\OSDA-DataManipulationAndManagement\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360753AE-6572-452C-AA7A-753B885F268B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDE892D-E9C9-4C41-ABD7-2BB2F869CAAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1204,7 +1204,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1214,6 +1214,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1272,7 +1278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1327,6 +1333,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1673,9 +1680,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1696,13 +1703,13 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="12" t="s">

</xml_diff>